<commit_message>
nearly there - backup
</commit_message>
<xml_diff>
--- a/Lookup File.xlsx
+++ b/Lookup File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KaranChauhan\Documents\Personal\PogoStatsLinear\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\UiPath\pkmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB04BC2-8478-45F6-A91C-FB6D29DE1D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B81939-DBDE-4C17-9455-A3671B8CE3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="-13245" windowWidth="18585" windowHeight="10695" xr2:uid="{9A9D2ED0-0B63-40EB-99D3-A09B524D4700}"/>
+    <workbookView xWindow="-11340" yWindow="-20640" windowWidth="38700" windowHeight="15285" xr2:uid="{9A9D2ED0-0B63-40EB-99D3-A09B524D4700}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Type</t>
   </si>
@@ -552,7 +552,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -767,7 +767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -777,8 +777,11 @@
       <c r="C18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>

</xml_diff>